<commit_message>
clean up columns in progress rpt
</commit_message>
<xml_diff>
--- a/progress report.xlsx
+++ b/progress report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="East" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="47">
   <si>
     <t>Team_Name</t>
   </si>
@@ -230,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -240,12 +240,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -587,18 +585,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J4" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,11 +618,8 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -656,7 +648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>6</v>
       </c>
@@ -685,7 +677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -714,7 +706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>14</v>
       </c>
@@ -743,7 +735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>10</v>
       </c>
@@ -772,7 +764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>9</v>
       </c>
@@ -801,7 +793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -830,7 +822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>12</v>
       </c>
@@ -858,14 +850,11 @@
       <c r="I9" s="4">
         <v>0</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="7">
         <v>42837</v>
       </c>
-      <c r="K9" s="9">
-        <v>42837</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -894,7 +883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -922,14 +911,11 @@
       <c r="I11" s="4">
         <v>0</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="7">
         <v>42833</v>
       </c>
-      <c r="K11" s="9">
-        <v>42833</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -957,49 +943,43 @@
       <c r="I12" s="4">
         <v>0</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="7">
         <v>42833</v>
       </c>
-      <c r="K12" s="9">
-        <v>42833</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
+    </row>
+    <row r="13" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
         <v>2</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="7">
+      <c r="D13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="6">
         <v>31</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>51</v>
       </c>
-      <c r="G13" s="7">
-        <v>0</v>
-      </c>
-      <c r="H13" s="7">
-        <v>1</v>
-      </c>
-      <c r="I13" s="7">
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1</v>
+      </c>
+      <c r="I13" s="6">
         <v>0</v>
       </c>
       <c r="J13" s="8">
-        <v>42822</v>
-      </c>
-      <c r="K13" s="10">
         <v>42823</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1027,14 +1007,11 @@
       <c r="I14">
         <v>0</v>
       </c>
-      <c r="J14" s="2">
-        <v>42822</v>
-      </c>
-      <c r="K14" s="11">
+      <c r="J14" s="9">
         <v>42823</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>3</v>
       </c>
@@ -1062,14 +1039,11 @@
       <c r="I15">
         <v>0</v>
       </c>
-      <c r="J15" s="2">
-        <v>42822</v>
-      </c>
-      <c r="K15" s="11">
+      <c r="J15" s="9">
         <v>42824</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -1097,10 +1071,7 @@
       <c r="I16">
         <v>0</v>
       </c>
-      <c r="J16" s="2">
-        <v>42802</v>
-      </c>
-      <c r="K16" s="11">
+      <c r="J16" s="9">
         <v>42801</v>
       </c>
     </row>
@@ -1111,19 +1082,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1148,11 +1118,8 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>20</v>
       </c>
@@ -1181,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>29</v>
       </c>
@@ -1210,7 +1177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>26</v>
       </c>
@@ -1239,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>19</v>
       </c>
@@ -1268,7 +1235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>21</v>
       </c>
@@ -1297,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>17</v>
       </c>
@@ -1326,7 +1293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>27</v>
       </c>
@@ -1355,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>18</v>
       </c>
@@ -1384,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>15</v>
       </c>
@@ -1412,14 +1379,11 @@
       <c r="I10" s="4">
         <v>0</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="7">
         <v>42834</v>
       </c>
-      <c r="K10" s="9">
-        <v>42834</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>28</v>
       </c>
@@ -1447,14 +1411,11 @@
       <c r="I11">
         <v>0</v>
       </c>
-      <c r="J11" s="2">
-        <v>42827</v>
-      </c>
-      <c r="K11" s="11">
+      <c r="J11" s="9">
         <v>42829</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>25</v>
       </c>
@@ -1482,14 +1443,11 @@
       <c r="I12" s="4">
         <v>0</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="7">
         <v>42826</v>
       </c>
-      <c r="K12" s="9">
-        <v>42826</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>24</v>
       </c>
@@ -1517,14 +1475,11 @@
       <c r="I13">
         <v>0</v>
       </c>
-      <c r="J13" s="2">
-        <v>42823</v>
-      </c>
-      <c r="K13" s="11">
+      <c r="J13" s="9">
         <v>42825</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>16</v>
       </c>
@@ -1552,14 +1507,11 @@
       <c r="I14" s="4">
         <v>0</v>
       </c>
-      <c r="J14" s="5">
-        <v>42826</v>
-      </c>
-      <c r="K14" s="9">
+      <c r="J14" s="7">
         <v>42827</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>22</v>
       </c>
@@ -1587,14 +1539,11 @@
       <c r="I15" s="4">
         <v>0</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="7">
         <v>42811</v>
       </c>
-      <c r="K15" s="9">
-        <v>42811</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>23</v>
       </c>
@@ -1622,10 +1571,7 @@
       <c r="I16">
         <v>0</v>
       </c>
-      <c r="J16" s="2">
-        <v>42815</v>
-      </c>
-      <c r="K16" s="11">
+      <c r="J16" s="9">
         <v>42816</v>
       </c>
     </row>

</xml_diff>